<commit_message>
2/3 of the class
</commit_message>
<xml_diff>
--- a/Session2_Ta/EXE2_input.xlsx
+++ b/Session2_Ta/EXE2_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sina\Documents\GitHub\Process-of-Organic-Industry--Spring-2024-\Session2_Ta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB95356C-5DEA-4549-99E9-0ABB2FC9893B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592139FE-B5F9-4449-AADB-82BE35BA2FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{6ED2B133-F318-4949-B732-FDB747F148CD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>K</t>
   </si>
@@ -247,12 +247,84 @@
   <si>
     <t>PROCESSES OF THE ORGANIC CHEMICAL INDUSTRY - TUTORIAL 2</t>
   </si>
+  <si>
+    <t>BOC</t>
+  </si>
+  <si>
+    <t>mol/s</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>nu M</t>
+  </si>
+  <si>
+    <t>nu R</t>
+  </si>
+  <si>
+    <t>ni 2</t>
+  </si>
+  <si>
+    <t>ni 1</t>
+  </si>
+  <si>
+    <t>lambda M</t>
+  </si>
+  <si>
+    <t>lambda R</t>
+  </si>
+  <si>
+    <t>MeOH</t>
+  </si>
+  <si>
+    <t>RWGS</t>
+  </si>
+  <si>
+    <t>Keq</t>
+  </si>
+  <si>
+    <t>Kp</t>
+  </si>
+  <si>
+    <t>Kphi</t>
+  </si>
+  <si>
+    <t>yi 2</t>
+  </si>
+  <si>
+    <t>needs a first assumption</t>
+  </si>
+  <si>
+    <t>Pi 2^ Num</t>
+  </si>
+  <si>
+    <t>Pi 2 ^ Nu RWGS</t>
+  </si>
+  <si>
+    <t>Pi 2 / pref</t>
+  </si>
+  <si>
+    <t>= Keq - Kp*Kphi = 0</t>
+  </si>
+  <si>
+    <t>Kp = product(Pi/Pref)^nu</t>
+  </si>
+  <si>
+    <t>IM, IG</t>
+  </si>
+  <si>
+    <t>Goal MeOH</t>
+  </si>
+  <si>
+    <t>Goal RWGS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,8 +385,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,8 +425,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -357,11 +459,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -398,9 +580,42 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -426,9 +641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>261406</xdr:colOff>
+      <xdr:colOff>261405</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>128345</xdr:rowOff>
+      <xdr:rowOff>96595</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -471,8 +686,8 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>400203</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>44020</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>202770</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -514,9 +729,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>520085</xdr:colOff>
+      <xdr:colOff>520086</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>145142</xdr:rowOff>
+      <xdr:rowOff>71058</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -558,9 +773,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>395625</xdr:colOff>
+      <xdr:colOff>395626</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>156991</xdr:rowOff>
+      <xdr:rowOff>8824</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -597,9 +812,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -637,7 +852,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -743,7 +958,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -885,7 +1100,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -893,15 +1108,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690D43F9-7A8B-4493-A597-005897D04447}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
@@ -915,7 +1138,7 @@
       <c r="I1" s="13"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -947,7 +1170,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -979,7 +1202,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1011,7 +1234,7 @@
         <v>0.22800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1043,7 +1266,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +1298,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1107,7 +1330,7 @@
         <v>0.56599999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1362,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
@@ -1171,7 +1394,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
@@ -1191,7 +1414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1201,8 +1424,17 @@
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1">
+        <v>100</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
@@ -1213,10 +1445,422 @@
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3">
+        <f xml:space="preserve"> $J$13*B4</f>
+        <v>5.4</v>
+      </c>
+      <c r="C17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <f xml:space="preserve"> B17+C17*$B$27+D17*$B$28</f>
+        <v>1.5756546323720637</v>
+      </c>
+      <c r="F17" s="3">
+        <f xml:space="preserve"> E17/$E$24</f>
+        <v>1.8145078325788058E-2</v>
+      </c>
+      <c r="G17" s="3">
+        <f xml:space="preserve"> F17*$F$12 / 1.015</f>
+        <v>1.4301539567123593</v>
+      </c>
+      <c r="H17" s="3">
+        <f xml:space="preserve"> G17^(C17)</f>
+        <v>0.69922541926800796</v>
+      </c>
+      <c r="I17" s="3">
+        <f xml:space="preserve"> G17^(D17)</f>
+        <v>1.4301539567123593</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" ref="B18:B23" si="0" xml:space="preserve"> $J$13*B5</f>
+        <v>10.08</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E18" s="3">
+        <f xml:space="preserve"> B18+C18*$B$27+D18*$B$28</f>
+        <v>7.3225826461278558</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" ref="F18:F23" si="1" xml:space="preserve"> E18/$E$24</f>
+        <v>8.4326116225748912E-2</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" ref="G18:G23" si="2" xml:space="preserve"> F18*$F$12 / 1.015</f>
+        <v>6.6463933971033633</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" ref="H18:H23" si="3" xml:space="preserve"> G18^(C18)</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" ref="I18:I23" si="4" xml:space="preserve"> G18^(D18)</f>
+        <v>0.15045753993975453</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>56.96</v>
+      </c>
+      <c r="C19" s="3">
+        <v>-2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="3">
+        <f xml:space="preserve"> B19+C19*$B$27+D19*$B$28</f>
+        <v>41.039057203127697</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="1"/>
+        <v>0.47260160448118477</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="2"/>
+        <v>37.249387545315059</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="3"/>
+        <v>7.2071195660305531E-4</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="4"/>
+        <v>2.6846078980049492E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <f xml:space="preserve"> B20+C20*$B$27+D20*$B$28</f>
+        <v>2.8474173538721446</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="1"/>
+        <v>3.2790568345829003E-2</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="2"/>
+        <v>2.5844782932673107</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5844782932673107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <f xml:space="preserve"> B21+C21*$B$27+D21*$B$28</f>
+        <v>7.0017627215000813</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="1"/>
+        <v>8.0631586637065683E-2</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="2"/>
+        <v>6.3551989467637986</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="3"/>
+        <v>6.3551989467637986</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>3.44</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <f xml:space="preserve"> B22+C22*$B$27+D22*$B$28</f>
+        <v>3.44</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="1"/>
+        <v>3.9614689766590758E-2</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="2"/>
+        <v>3.1223400801253804</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>23.61</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <f xml:space="preserve"> B23+C23*$B$27+D23*$B$28</f>
+        <v>23.61</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="1"/>
+        <v>0.27189035621779295</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="2"/>
+        <v>21.429781770860529</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="22">
+        <f xml:space="preserve"> SUM(B17:B23)</f>
+        <v>100</v>
+      </c>
+      <c r="C24" s="23">
+        <f xml:space="preserve"> SUM(C17:C23)</f>
+        <v>-2</v>
+      </c>
+      <c r="D24" s="23">
+        <f xml:space="preserve"> SUM(D17:D23)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="23">
+        <f xml:space="preserve"> SUM(E17:E23)</f>
+        <v>86.836474556999832</v>
+      </c>
+      <c r="F24" s="23">
+        <f xml:space="preserve"> SUM(F17:F23)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="G24" s="23">
+        <f xml:space="preserve"> SUM(G17:G23)</f>
+        <v>78.817733990147815</v>
+      </c>
+      <c r="H24" s="23">
+        <f t="shared" ref="H24:I24" si="5" xml:space="preserve"> SUM(H17:H23)</f>
+        <v>11.05514507798841</v>
+      </c>
+      <c r="I24" s="23">
+        <f t="shared" si="5"/>
+        <v>7.1919358688994741</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="16">
+        <v>6.5817627215000813</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="16">
+        <v>2.7574173538721447</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="3">
+        <f xml:space="preserve"> EXP(-(-22828+56.02*B13)/1.987/B13)</f>
+        <v>1.4788237850626839E-3</v>
+      </c>
+      <c r="K28" s="3">
+        <f xml:space="preserve"> PRODUCT(H17:H23)</f>
+        <v>3.2026397200291237E-3</v>
+      </c>
+      <c r="L28" s="3">
+        <v>1</v>
+      </c>
+      <c r="M28" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I29" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="3">
+        <f xml:space="preserve"> EXP(-(8514-7.71*B13)/1.987/B13)</f>
+        <v>1.4929680039997966E-2</v>
+      </c>
+      <c r="K29" s="3">
+        <f xml:space="preserve"> PRODUCT(I17:I23)</f>
+        <v>1.4929680061759961E-2</v>
+      </c>
+      <c r="L29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I31" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>46</v>
+      </c>
+      <c r="L32">
+        <f xml:space="preserve"> LN(J28)-LN(K28*L28)</f>
+        <v>-0.77272835028105646</v>
+      </c>
+    </row>
+    <row r="33" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>47</v>
+      </c>
+      <c r="L33">
+        <f xml:space="preserve"> LN(J29) -LN(K29*L29)</f>
+        <v>-1.4576331253124408E-9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A26:C26"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>